<commit_message>
Update after meeting with Heather
</commit_message>
<xml_diff>
--- a/datasets/distiller_cross.xlsx
+++ b/datasets/distiller_cross.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate-my.sharepoint.com/personal/fonsec16_msu_edu/Documents/Documents/CAFO-July-2021/Update-Website-July-2021/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="139" documentId="8_{42FCA062-115A-4175-8F63-773B4F4DB047}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{132760FD-D63B-49DD-9767-7F4E9F999446}"/>
+  <xr:revisionPtr revIDLastSave="145" documentId="8_{42FCA062-115A-4175-8F63-773B4F4DB047}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C1B5C7D3-36B0-4BBF-AC76-AEA2975BC327}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:BM112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F107" sqref="F107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -10685,7 +10685,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="108" spans="1:65" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>303</v>
       </c>
@@ -10783,7 +10783,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="109" spans="1:65" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>303</v>
       </c>
@@ -10887,7 +10887,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="110" spans="1:65" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>303</v>
       </c>
@@ -10979,7 +10979,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="111" spans="1:65" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>303</v>
       </c>
@@ -11095,7 +11095,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="112" spans="1:65" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>303</v>
       </c>
@@ -11201,9 +11201,10 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:BM112" xr:uid="{88636C4F-9030-4648-BA6D-129EFCDC7523}">
-    <filterColumn colId="5">
+    <filterColumn colId="0">
       <filters>
-        <filter val="Antimicrobial resistance"/>
+        <filter val="32507530"/>
+        <filter val="32507767"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>